<commit_message>
Added java code with new exception classes
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -16,15 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Operations</t>
-  </si>
-  <si>
-    <t>CraftMan</t>
-  </si>
-  <si>
-    <t>Client</t>
   </si>
   <si>
     <t>Resource</t>
@@ -34,6 +28,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Users</t>
   </si>
 </sst>
 </file>
@@ -69,13 +66,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -101,12 +95,12 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4130040</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -151,70 +145,6 @@
         <a:bodyPr wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Register</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Login</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Logout</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Delete</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t> Account</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Edit Account</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Create profile</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Add Categories</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Candidate for Offers</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Search offers/by category</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Sort offers/by category</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="bg-BG" sz="1100" b="1"/>
         </a:p>
       </xdr:txBody>
@@ -225,13 +155,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4114800</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -322,6 +252,36 @@
             </a:rPr>
             <a:t>Logout</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Edit Account</a:t>
+          </a:r>
           <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
         </a:p>
         <a:p>
@@ -343,12 +303,6 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Comment craftman profile</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
             <a:t>Rate craftman profile</a:t>
           </a:r>
         </a:p>
@@ -363,6 +317,9 @@
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
             <a:t>Sort craftmen/by rating/by date registered</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="bg-BG" sz="1100" b="1"/>
@@ -375,13 +332,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4107180</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>1318260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -428,35 +385,41 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Add tittle</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Select</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t> category</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Add maximum budget</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Add description</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>Add pictures</a:t>
+            <a:t>Add</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t> offer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Edit offer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Delete offer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Get my offers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Get all offers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Filter offers/by date added/</a:t>
           </a:r>
           <a:endParaRPr lang="bg-BG" sz="1100" b="1"/>
         </a:p>
@@ -468,13 +431,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4091940</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>1280160</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -530,19 +493,6 @@
             <a:t>Edit comment</a:t>
           </a:r>
         </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
-            <a:t>Reply</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t> on comment</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="bg-BG" sz="1100" b="1"/>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -551,8 +501,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Resource" dataDxfId="0"/>
     <tableColumn id="2" name="Operations"/>
@@ -846,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -861,33 +811,27 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="160.80000000000001" customHeight="1">
+    <row r="2" spans="1:2" ht="142.80000000000001" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
-      <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="149.4" customHeight="1">
+    <row r="3" spans="1:2" ht="95.4" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="106.8" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
+    <row r="4" spans="1:2" ht="39" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="54.6" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4"/>
+      <c r="B4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new row in rating table
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4D956F-5736-46CC-9539-A29333641480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,8 +42,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,10 +87,18 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -105,7 +119,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -166,7 +186,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -207,13 +233,21 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Register</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Login</a:t>
           </a:r>
         </a:p>
@@ -274,7 +308,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -282,21 +316,37 @@
             </a:rPr>
             <a:t>Edit Account</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Delete</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t> Account</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Post offers</a:t>
           </a:r>
         </a:p>
@@ -343,7 +393,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -442,7 +498,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -501,11 +563,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Resource" dataDxfId="0"/>
-    <tableColumn id="2" name="Operations"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Resource" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Operations"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -554,7 +616,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -586,9 +648,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -620,6 +700,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -795,21 +893,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="60.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -817,17 +915,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="142.80000000000001" customHeight="1">
+    <row r="2" spans="1:2" ht="142.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="95.4" customHeight="1">
+    <row r="3" spans="1:2" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" customHeight="1">
+    <row r="4" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -844,24 +942,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added username and password validations
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4D956F-5736-46CC-9539-A29333641480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC28B336-8B8B-498A-AA97-D6E5684F42CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,7 +275,7 @@
                 <a:noFill/>
               </a:ln>
               <a:solidFill>
-                <a:prstClr val="black"/>
+                <a:srgbClr val="FFFF00"/>
               </a:solidFill>
               <a:effectLst/>
               <a:uLnTx/>
@@ -338,16 +338,6 @@
               </a:solidFill>
             </a:rPr>
             <a:t> Account</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Post offers</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -440,29 +430,49 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Add</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t> offer</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Edit offer</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Delete offer</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Get my offers</a:t>
           </a:r>
         </a:p>
@@ -897,7 +907,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new commit for check
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC28B336-8B8B-498A-AA97-D6E5684F42CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6F047D-E5CD-4CD7-9590-70948C927DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Operations</t>
   </si>
@@ -38,17 +38,35 @@
   <si>
     <t>Users</t>
   </si>
+  <si>
+    <t>Job Done</t>
+  </si>
+  <si>
+    <t>Job Left</t>
+  </si>
+  <si>
+    <t>№</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -72,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -81,6 +99,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,7 +256,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>Register</a:t>
@@ -245,7 +266,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>Login</a:t>
@@ -275,7 +296,7 @@
                 <a:noFill/>
               </a:ln>
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:effectLst/>
               <a:uLnTx/>
@@ -308,7 +329,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -318,7 +339,7 @@
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100" b="1">
             <a:solidFill>
-              <a:srgbClr val="FFFF00"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -326,7 +347,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>Delete</a:t>
@@ -334,7 +355,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
             </a:rPr>
             <a:t> Account</a:t>
@@ -342,7 +363,11 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Rate craftman profile</a:t>
           </a:r>
         </a:p>
@@ -470,7 +495,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
+                <a:srgbClr val="92D050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>Get my offers</a:t>
@@ -906,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,13 +978,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added Comment and Add and Edit Methods
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6F047D-E5CD-4CD7-9590-70948C927DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1862D13E-D8E7-4D78-89C6-6C2E6761845E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -580,7 +580,11 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Add comment</a:t>
           </a:r>
         </a:p>
@@ -931,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -980,7 +984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished comments and added some method for categories
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1862D13E-D8E7-4D78-89C6-6C2E6761845E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEE0C31-C2F9-4D63-AD66-3DD1433B39AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Operations</t>
   </si>
@@ -46,13 +46,139 @@
   </si>
   <si>
     <t>№</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Resourse</t>
+  </si>
+  <si>
+    <t>Request_Type</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>getById</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>deleteById</t>
+  </si>
+  <si>
+    <t>EditAccount</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>addComment</t>
+  </si>
+  <si>
+    <t>editComment</t>
+  </si>
+  <si>
+    <t>getAllCommentByOwnerID</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>rateCraftsman</t>
+  </si>
+  <si>
+    <t>editRate</t>
+  </si>
+  <si>
+    <t>unrateCraftsman</t>
+  </si>
+  <si>
+    <t>getAverageRate</t>
+  </si>
+  <si>
+    <t>postOffer</t>
+  </si>
+  <si>
+    <t>findById</t>
+  </si>
+  <si>
+    <t>editOffer</t>
+  </si>
+  <si>
+    <t>deleteOffer</t>
+  </si>
+  <si>
+    <t>getAllOffers</t>
+  </si>
+  <si>
+    <t>getAllOffersForUser</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>editCategory</t>
+  </si>
+  <si>
+    <t>deleteCategory</t>
+  </si>
+  <si>
+    <t>getAllCategories</t>
+  </si>
+  <si>
+    <t>getAllByCity</t>
+  </si>
+  <si>
+    <t>getAllByCategory</t>
+  </si>
+  <si>
+    <t>getCraftsmanByCategory</t>
+  </si>
+  <si>
+    <t>getCraftsmanByCity</t>
+  </si>
+  <si>
+    <t>getAllCraftsmans</t>
+  </si>
+  <si>
+    <t>getAllUsers</t>
+  </si>
+  <si>
+    <t>uploadPhoto</t>
+  </si>
+  <si>
+    <t>addCategory</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>getCommentById</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +195,37 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -86,11 +233,227 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -102,6 +465,121 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +1068,11 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Edit comment</a:t>
           </a:r>
         </a:p>
@@ -935,7 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1104,12 +1586,228 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+      <c r="B7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="40"/>
+      <c r="B9" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
+      <c r="B15" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add many to many relationship, addCategory method
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEE0C31-C2F9-4D63-AD66-3DD1433B39AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A24C7C-33E6-4474-A4A0-0D5D15E16861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,20 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Operations</t>
   </si>
@@ -465,20 +473,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,19 +519,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,18 +533,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,6 +551,45 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,9 +1015,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4091940</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1280160</xdr:rowOff>
+      <xdr:colOff>4025265</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6437</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1022,8 +1032,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2369820" y="4488180"/>
-          <a:ext cx="4053840" cy="1249680"/>
+          <a:off x="2304393" y="3242704"/>
+          <a:ext cx="3987165" cy="468630"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1418,7 +1428,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1599,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,200 +1612,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="25" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="43"/>
+      <c r="B5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="43"/>
+      <c r="B6" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
+      <c r="C7" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="32" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="46" t="s">
+      <c r="A9" s="46"/>
+      <c r="B9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="8"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="29" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="42"/>
+      <c r="B12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="42"/>
+      <c r="B13" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="23"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="42"/>
+      <c r="B14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="36" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added admin role, added delete craftsman category
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A24C7C-33E6-4474-A4A0-0D5D15E16861}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20FD216-C547-4358-AD37-AD2C7487E8B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Primary_version" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Modified_Action_Plan" sheetId="3" r:id="rId3"/>
+    <sheet name="Schedule_For_Presentation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>Operations</t>
   </si>
@@ -180,6 +181,39 @@
   </si>
   <si>
     <t>getCommentById</t>
+  </si>
+  <si>
+    <t>addCraftsmanCategory</t>
+  </si>
+  <si>
+    <t>deleteCraftsmanCategory</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>register craftsman</t>
+  </si>
+  <si>
+    <t>login accepted/failed</t>
+  </si>
+  <si>
+    <t>register user accepted/failed</t>
+  </si>
+  <si>
+    <t>upload photo</t>
+  </si>
+  <si>
+    <t>add offer</t>
+  </si>
+  <si>
+    <t>add comment to offer</t>
+  </si>
+  <si>
+    <t>rate craftsman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add craftsman category </t>
   </si>
 </sst>
 </file>
@@ -557,6 +591,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -586,9 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1598,32 +1632,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1672,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1655,7 +1689,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="14" t="s">
         <v>42</v>
       </c>
@@ -1664,22 +1698,22 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="25" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="14" t="s">
         <v>44</v>
       </c>
@@ -1690,18 +1724,18 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>47</v>
+      <c r="C7" s="37" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="46" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="30" t="s">
@@ -1718,7 +1752,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="33" t="s">
         <v>49</v>
       </c>
@@ -1744,7 +1778,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="42" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1761,7 +1795,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="16" t="s">
         <v>34</v>
       </c>
@@ -1770,7 +1804,7 @@
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="16" t="s">
         <v>35</v>
       </c>
@@ -1779,7 +1813,7 @@
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="16" t="s">
         <v>40</v>
       </c>
@@ -1788,7 +1822,7 @@
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="20" t="s">
         <v>41</v>
       </c>
@@ -1824,4 +1858,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195710B0-343F-4B53-BB8A-79C92A1E2979}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit for merging(nothing changed)
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20FD216-C547-4358-AD37-AD2C7487E8B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56525CEE-A233-4ADC-880F-28DF88341878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_version" sheetId="1" r:id="rId1"/>
@@ -1461,7 +1461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1633,7 +1633,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,7 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195710B0-343F-4B53-BB8A-79C92A1E2979}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finished end point of offer application and few other changes
</commit_message>
<xml_diff>
--- a/Action Plan.xlsx
+++ b/Action Plan.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Coding\IT_Talents_Season_14_Java1\Test3\Final_Project\S14_MAISTOR_BG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56525CEE-A233-4ADC-880F-28DF88341878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B81062-873D-4B93-872C-D382701D6117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_version" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="WorkLeft" sheetId="2" r:id="rId2"/>
     <sheet name="Modified_Action_Plan" sheetId="3" r:id="rId3"/>
     <sheet name="Schedule_For_Presentation" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>Operations</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Users</t>
   </si>
   <si>
-    <t>Job Done</t>
-  </si>
-  <si>
     <t>Job Left</t>
   </si>
   <si>
@@ -214,6 +211,57 @@
   </si>
   <si>
     <t xml:space="preserve">add craftsman category </t>
+  </si>
+  <si>
+    <t>Is done?</t>
+  </si>
+  <si>
+    <t>Да се направи заявка за показване на всички подкоментари към коментар</t>
+  </si>
+  <si>
+    <t>Да се проверят Postman body-тата дали отговарят на промените</t>
+  </si>
+  <si>
+    <t>Проверка при кандидатстване за обява, дали обява е затворена</t>
+  </si>
+  <si>
+    <t>Да се прегледат и преработят DTO-тата на Offer</t>
+  </si>
+  <si>
+    <t>Да се добавят валидации за логнат user или owner при новите методи за кандидатстване към обява</t>
+  </si>
+  <si>
+    <t>Останалите статистики от action plan таблицата</t>
+  </si>
+  <si>
+    <t>Изпробване на всички Postman заявки</t>
+  </si>
+  <si>
+    <t>Изготвяне на Postman план за представяне във вторник</t>
+  </si>
+  <si>
+    <t>Презентация</t>
+  </si>
+  <si>
+    <t>Unit tests/send verification email, при евентуално останало време</t>
+  </si>
+  <si>
+    <t>Преглеждане отново на кода и рефактор</t>
+  </si>
+  <si>
+    <t>CronJob, който да върти през определено време и да проверява за обяви с изтекъл срок</t>
+  </si>
+  <si>
+    <t>Индекси където търсим по колона различна от ID-то</t>
+  </si>
+  <si>
+    <t>Да се добави да може да се трие коментар и проверка при триене на коментар дали човека е собственик на коментара</t>
+  </si>
+  <si>
+    <t>При добавяне на обява да се преработи да се сетва duration-a</t>
+  </si>
+  <si>
+    <t>Да се добави logout-ване при определена неактивност</t>
   </si>
 </sst>
 </file>
@@ -247,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +314,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -495,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,6 +678,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,7 +1098,11 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Get all offers</a:t>
           </a:r>
         </a:p>
@@ -1461,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1508,119 +1585,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="50">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="48" t="s">
+        <v>61</v>
+      </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="48" t="s">
+        <v>62</v>
+      </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="50">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="48" t="s">
+        <v>64</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="50">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="50" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="49" t="s">
+        <v>66</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="49" t="s">
+        <v>67</v>
+      </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="48" t="s">
+        <v>68</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="49" t="s">
+        <v>69</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="48" t="s">
+        <v>72</v>
+      </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="49" t="s">
+        <v>71</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="52">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="54"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="50">
+        <v>15</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1633,7 +1769,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,10 +1783,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>10</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -1659,55 +1795,55 @@
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
       <c r="B2" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
@@ -1715,10 +1851,10 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
@@ -1726,35 +1862,35 @@
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>23</v>
-      </c>
       <c r="E8" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
       <c r="B9" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="34"/>
@@ -1762,19 +1898,19 @@
     </row>
     <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="28" t="s">
+      <c r="D10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="E10" s="29" t="s">
         <v>27</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,22 +1918,22 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="43"/>
       <c r="B12" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1806,7 +1942,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="43"/>
       <c r="B13" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -1815,7 +1951,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
       <c r="B14" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -1824,7 +1960,7 @@
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="45"/>
       <c r="B15" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -1832,19 +1968,19 @@
     </row>
     <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="35" t="s">
+      <c r="E16" s="36" t="s">
         <v>37</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1875,10 +2011,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1886,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1894,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1902,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1910,7 +2046,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +2054,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1926,7 +2062,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1934,7 +2070,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +2078,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>